<commit_message>
se realiza la funcion registrarDatos donde permite validar que id se debe registrar
</commit_message>
<xml_diff>
--- a/reportes/davivienda.xlsx
+++ b/reportes/davivienda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Diana\reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{230DE905-3B5F-47EE-8E2F-F845E0ADC3E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3849EF57-69EB-499E-AADB-7476B7937224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{2AA892C9-49D5-419C-9581-2C5FCC6E06B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A44ED20B-6B96-40E0-8BE3-6146AAF220F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B1DD2-F5B4-4D2A-B581-E11A0A9E0027}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93A2C01-1E75-4DDC-B0B0-A201BA64734F}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>